<commit_message>
Updated USA model - 2025-08-03 12:38
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/SuppXLS/scen_tsparameters_ts_2weeks.xlsx
+++ b/VerveStacks_USA/SuppXLS/scen_tsparameters_ts_2weeks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9723B6-FF32-4BF6-A26B-2BDBE3D67FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7AC52C-8282-451E-BA45-DED171A94D30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -1071,10 +1071,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>S3aH3,S6c1203h09,S6aH5,S3aH4,S4aH3,S4aH4,S6b0924h09,S6c1209h15,S1aH2,S2aH3,S3aH6,S5aH6,S6aH6,S6c1209h13,S6c1209h16,S4aH2,S6b0924h11,S6c1203h08,S6c1203h10,S6c1209h09,S6c1209h10,S4aH5,S6b0924h10,S6b0924h13,S6b0924h16,S6b0930h07,S6b0930h09,S6c1203h12,S6b0924h08,S6b0924h12,S6b0924h18,S6b0930h11,S6c1209h08,S6c1209h18,S1aH6,S6b0930h10,S2aH6,S3aH5,S5aH3,S6b0924h15,S3aH2,S6c1203h15,S1aH3,S6b0924h07,S6b0924h14,S6b0930h18,S6c1203h18,S1aH4,S2aH2,S4aH6,S6b0930h17,S6c1209h12,S5aH4,S6aH3,S6aH4,S6c1203h13,S6c1203h14,S6c1209h14,S6c1209h17,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S6b0924h17,S6b0930h12,S6c1203h07,S6c1203h16,S6b0930h13,S6b0930h14,S6c1203h11,S6c1209h07,S6b0930h08,S6b0930h15,S6b0930h16,S6c1203h17,S6c1209h11</t>
-  </si>
-  <si>
-    <t>S6c1203h01,S4aH8,S6b0924h06,S6b0924h24,S6b0930h19,S6c1203h06,S6c1209h06,S6c1209h24,S6b0924h20,S6b0924h05,S6b0930h22,S6c1203h04,S6c1209h20,S2aH1,S3aH7,S5aH8,S6c1203h21,S6c1209h02,S6b0924h01,S6b0930h06,S6b0930h21,S6c1209h21,S3aH1,S6b0930h20,S6c1209h01,S6aH8,S6b0924h03,S6c1203h03,S6c1203h23,S1aH8,S5aH1,S6aH7,S6b0930h23,S6c1209h19,S6c1209h22,S3aH8,S6b0924h22,S6b0924h23,S6b0930h01,S6c1203h02,S6c1209h04,S1aH7,S4aH7,S5aH7,S6b0924h04,S6c1203h20,S4aH1,S6aH1,S6c1203h22,S6b0924h02,S6b0924h21,S6c1203h19,S6c1203h24,S6b0930h03,S6c1203h05,S6c1209h23,S2aH8,S6b0930h04,S6c1209h03,S6c1209h05,S1aH1,S2aH7,S6b0924h19,S6b0930h02,S6b0930h05,S6b0930h24</t>
+    <t>S6b0930h13,S6b0930h14,S6c1203h11,S6c1209h07,S5aH4,S6aH3,S6aH4,S6c1203h13,S6c1203h14,S6c1209h14,S6c1209h17,S6aH5,S6b0930h08,S6b0930h15,S6b0930h16,S6c1203h17,S6c1209h11,S4aH5,S6b0924h10,S6b0924h13,S6b0924h16,S6b0930h07,S6b0930h09,S6c1203h12,S2aH6,S3aH5,S5aH3,S6b0924h15,S4aH2,S6b0924h11,S6c1203h08,S6c1203h10,S6c1209h09,S6c1209h10,S3aH3,S6c1203h09,S3aH2,S6c1203h15,S1aH4,S2aH2,S4aH6,S6b0930h17,S6c1209h12,S1aH2,S2aH3,S3aH6,S5aH6,S6aH6,S6c1209h13,S6c1209h16,S1aH6,S6b0930h10,S6b0924h08,S6b0924h12,S6b0924h18,S6b0930h11,S6c1209h08,S6c1209h18,S1aH3,S6b0924h07,S6b0924h14,S6b0930h18,S6c1203h18,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S6b0924h17,S6b0930h12,S6c1203h07,S6c1203h16,S3aH4,S4aH3,S4aH4,S6b0924h09,S6c1209h15</t>
+  </si>
+  <si>
+    <t>S2aH8,S6b0930h04,S6c1209h03,S6c1209h05,S6b0924h02,S6b0924h21,S6c1203h19,S6c1203h24,S4aH8,S6b0924h06,S6b0924h24,S6b0930h19,S6c1203h06,S6c1209h06,S6c1209h24,S1aH1,S2aH7,S6b0924h19,S6b0930h02,S6b0930h05,S6b0930h24,S6b0924h01,S6b0930h06,S6b0930h21,S6c1209h21,S1aH8,S5aH1,S6aH7,S6b0930h23,S6c1209h19,S6c1209h22,S2aH1,S3aH7,S5aH8,S6c1203h21,S6c1209h02,S6c1203h01,S3aH8,S6b0924h22,S6b0924h23,S6b0930h01,S6c1203h02,S6c1209h04,S4aH1,S6aH1,S6c1203h22,S6b0924h05,S6b0930h22,S6c1203h04,S6c1209h20,S6aH8,S6b0924h03,S6c1203h03,S6c1203h23,S3aH1,S6b0930h20,S6c1209h01,S1aH7,S4aH7,S5aH7,S6b0924h04,S6c1203h20,S6b0930h03,S6c1203h05,S6c1209h23,S6b0924h20</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1645,7 +1645,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>S6c1203h01,S4aH8,S6b0924h06,S6b0924h24,S6b0930h19,S6c1203h06,S6c1209h06,S6c1209h24,S6b0924h20,S6b0924h05,S6b0930h22,S6c1203h04,S6c1209h20,S2aH1,S3aH7,S5aH8,S6c1203h21,S6c1209h02,S6b0924h01,S6b0930h06,S6b0930h21,S6c1209h21,S3aH1,S6b0930h20,S6c1209h01,S6aH8,S6b0924h03,S6c1203h03,S6c1203h23,S1aH8,S5aH1,S6aH7,S6b0930h23,S6c1209h19,S6c1209h22,S3aH8,S6b0924h22,S6b0924h23,S6b0930h01,S6c1203h02,S6c1209h04,S1aH7,S4aH7,S5aH7,S6b0924h04,S6c1203h20,S4aH1,S6aH1,S6c1203h22,S6b0924h02,S6b0924h21,S6c1203h19,S6c1203h24,S6b0930h03,S6c1203h05,S6c1209h23,S2aH8,S6b0930h04,S6c1209h03,S6c1209h05,S1aH1,S2aH7,S6b0924h19,S6b0930h02,S6b0930h05,S6b0930h24</v>
+        <v>S2aH8,S6b0930h04,S6c1209h03,S6c1209h05,S6b0924h02,S6b0924h21,S6c1203h19,S6c1203h24,S4aH8,S6b0924h06,S6b0924h24,S6b0930h19,S6c1203h06,S6c1209h06,S6c1209h24,S1aH1,S2aH7,S6b0924h19,S6b0930h02,S6b0930h05,S6b0930h24,S6b0924h01,S6b0930h06,S6b0930h21,S6c1209h21,S1aH8,S5aH1,S6aH7,S6b0930h23,S6c1209h19,S6c1209h22,S2aH1,S3aH7,S5aH8,S6c1203h21,S6c1209h02,S6c1203h01,S3aH8,S6b0924h22,S6b0924h23,S6b0930h01,S6c1203h02,S6c1209h04,S4aH1,S6aH1,S6c1203h22,S6b0924h05,S6b0930h22,S6c1203h04,S6c1209h20,S6aH8,S6b0924h03,S6c1203h03,S6c1203h23,S3aH1,S6b0930h20,S6c1209h01,S1aH7,S4aH7,S5aH7,S6b0924h04,S6c1203h20,S6b0930h03,S6c1203h05,S6c1209h23,S6b0924h20</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>S3aH3,S6c1203h09,S6aH5,S3aH4,S4aH3,S4aH4,S6b0924h09,S6c1209h15,S1aH2,S2aH3,S3aH6,S5aH6,S6aH6,S6c1209h13,S6c1209h16,S4aH2,S6b0924h11,S6c1203h08,S6c1203h10,S6c1209h09,S6c1209h10,S4aH5,S6b0924h10,S6b0924h13,S6b0924h16,S6b0930h07,S6b0930h09,S6c1203h12,S6b0924h08,S6b0924h12,S6b0924h18,S6b0930h11,S6c1209h08,S6c1209h18,S1aH6,S6b0930h10,S2aH6,S3aH5,S5aH3,S6b0924h15,S3aH2,S6c1203h15,S1aH3,S6b0924h07,S6b0924h14,S6b0930h18,S6c1203h18,S1aH4,S2aH2,S4aH6,S6b0930h17,S6c1209h12,S5aH4,S6aH3,S6aH4,S6c1203h13,S6c1203h14,S6c1209h14,S6c1209h17,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S6b0924h17,S6b0930h12,S6c1203h07,S6c1203h16,S6b0930h13,S6b0930h14,S6c1203h11,S6c1209h07,S6b0930h08,S6b0930h15,S6b0930h16,S6c1203h17,S6c1209h11</v>
+        <v>S6b0930h13,S6b0930h14,S6c1203h11,S6c1209h07,S5aH4,S6aH3,S6aH4,S6c1203h13,S6c1203h14,S6c1209h14,S6c1209h17,S6aH5,S6b0930h08,S6b0930h15,S6b0930h16,S6c1203h17,S6c1209h11,S4aH5,S6b0924h10,S6b0924h13,S6b0924h16,S6b0930h07,S6b0930h09,S6c1203h12,S2aH6,S3aH5,S5aH3,S6b0924h15,S4aH2,S6b0924h11,S6c1203h08,S6c1203h10,S6c1209h09,S6c1209h10,S3aH3,S6c1203h09,S3aH2,S6c1203h15,S1aH4,S2aH2,S4aH6,S6b0930h17,S6c1209h12,S1aH2,S2aH3,S3aH6,S5aH6,S6aH6,S6c1209h13,S6c1209h16,S1aH6,S6b0930h10,S6b0924h08,S6b0924h12,S6b0924h18,S6b0930h11,S6c1209h08,S6c1209h18,S1aH3,S6b0924h07,S6b0924h14,S6b0930h18,S6c1203h18,S1aH5,S2aH4,S2aH5,S5aH2,S5aH5,S6aH2,S6b0924h17,S6b0930h12,S6c1203h07,S6c1203h16,S3aH4,S4aH3,S4aH4,S6b0924h09,S6c1209h15</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2290,7 +2290,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD4979AE-A992-484C-86B8-55CA97345484}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79D1CEB5-96AB-43BB-852D-98439CFD9F1A}">
   <dimension ref="B2:F107"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3193,7 +3193,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5447E94F-81DC-4D7E-9A9D-1BECB5BF17DE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D155340-6A5D-48FC-825C-FAD83759222E}">
   <dimension ref="B2:O147"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3272,10 +3272,10 @@
         <v>194</v>
       </c>
       <c r="M4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="N4">
-        <v>0.10830924286565957</v>
+        <v>9.560747348173812E-2</v>
       </c>
       <c r="O4" t="s">
         <v>350</v>
@@ -3307,10 +3307,10 @@
         <v>194</v>
       </c>
       <c r="M5" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="N5">
-        <v>9.560747348173812E-2</v>
+        <v>0.24201623957307244</v>
       </c>
       <c r="O5" t="s">
         <v>350</v>
@@ -3342,10 +3342,10 @@
         <v>194</v>
       </c>
       <c r="M6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N6">
-        <v>0.10847507741355956</v>
+        <v>0.10830924286565957</v>
       </c>
       <c r="O6" t="s">
         <v>350</v>
@@ -3377,10 +3377,10 @@
         <v>194</v>
       </c>
       <c r="M7" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="N7">
-        <v>0.24201623957307244</v>
+        <v>0.53877330642271426</v>
       </c>
       <c r="O7" t="s">
         <v>350</v>
@@ -3412,10 +3412,10 @@
         <v>194</v>
       </c>
       <c r="M8" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="N8">
-        <v>0.10681866024325613</v>
+        <v>0.10847507741355956</v>
       </c>
       <c r="O8" t="s">
         <v>350</v>
@@ -3447,10 +3447,10 @@
         <v>194</v>
       </c>
       <c r="M9" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="N9">
-        <v>0.53877330642271426</v>
+        <v>0.10681866024325613</v>
       </c>
       <c r="O9" t="s">
         <v>350</v>
@@ -7050,7 +7050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239D04A4-394B-41BE-ADA9-47FB2838731C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{696261EF-3E9F-4FEB-A6FB-6ED6FC71FE54}">
   <dimension ref="B2:O291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated USA model - 2025-08-03 17:49
</commit_message>
<xml_diff>
--- a/VerveStacks_USA/SuppXLS/scen_tsparameters_ts_2weeks.xlsx
+++ b/VerveStacks_USA/SuppXLS/scen_tsparameters_ts_2weeks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_USA\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83A051FD-D279-4C0B-BDA3-C5502594BDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47655EDA-332F-4D83-8794-92D4E5C45D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -3730,7 +3730,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA533F2-FC75-492C-960E-1958F3F2A049}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60A75613-571A-4095-8C60-D9A85BC736B7}">
   <dimension ref="B2:F347"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6553,7 +6553,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE2F8CE8-C9D3-4B03-A45A-4B82A1D62D2C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60E7BC02-D864-42F7-AFCD-9E773B873AAF}">
   <dimension ref="B2:O387"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6632,10 +6632,10 @@
         <v>434</v>
       </c>
       <c r="M4" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="N4">
-        <v>9.5607473481738106E-2</v>
+        <v>0.10681866024325613</v>
       </c>
       <c r="O4" t="s">
         <v>830</v>
@@ -6670,7 +6670,7 @@
         <v>87</v>
       </c>
       <c r="N5">
-        <v>0.24201623957307239</v>
+        <v>0.24201623957307244</v>
       </c>
       <c r="O5" t="s">
         <v>830</v>
@@ -6705,7 +6705,7 @@
         <v>82</v>
       </c>
       <c r="N6">
-        <v>0.53877330642271404</v>
+        <v>0.53877330642271426</v>
       </c>
       <c r="O6" t="s">
         <v>830</v>
@@ -6740,7 +6740,7 @@
         <v>83</v>
       </c>
       <c r="N7">
-        <v>0.10830924286565956</v>
+        <v>0.10830924286565957</v>
       </c>
       <c r="O7" t="s">
         <v>830</v>
@@ -6772,10 +6772,10 @@
         <v>434</v>
       </c>
       <c r="M8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N8">
-        <v>0.10847507741355955</v>
+        <v>9.560747348173812E-2</v>
       </c>
       <c r="O8" t="s">
         <v>830</v>
@@ -6807,10 +6807,10 @@
         <v>434</v>
       </c>
       <c r="M9" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="N9">
-        <v>0.10681866024325611</v>
+        <v>0.10847507741355956</v>
       </c>
       <c r="O9" t="s">
         <v>830</v>
@@ -16650,7 +16650,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECF3FE5-EE36-4351-98E4-E68705B4581B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{150D7F8C-C712-48C4-8846-BF19353FCD5D}">
   <dimension ref="B2:O771"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>